<commit_message>
updated to selenium 4.11 and code fix
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestData.xlsx
+++ b/src/test/resources/data/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Space\workspace\eclipse-workspace\DataDrivenTesting-Sample\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\java\DataDrivenFramework_v2-sample\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE03CB3-F91B-470F-B651-0E7BA86AB36E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708E64EF-FA5F-436D-8E7A-6463F418AA68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="253">
   <si>
     <t>Description</t>
   </si>
@@ -353,9 +353,6 @@
     <t>6011111111111117</t>
   </si>
   <si>
-    <t>07-2022</t>
-  </si>
-  <si>
     <t>Genuine Leather Handbag</t>
   </si>
   <si>
@@ -789,6 +786,12 @@
   </si>
   <si>
     <t>There is NO data sheet for this test.</t>
+  </si>
+  <si>
+    <t>07-2025</t>
+  </si>
+  <si>
+    <t>10-2024</t>
   </si>
 </sst>
 </file>
@@ -853,7 +856,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -883,9 +886,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1172,19 +1172,19 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D2" sqref="D2:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1"/>
+    <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.44140625" customWidth="1"/>
     <col min="3" max="3" width="68" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="56.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1257,91 +1257,91 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" t="s">
         <v>112</v>
-      </c>
-      <c r="C6" t="s">
-        <v>113</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C9" t="s">
         <v>164</v>
-      </c>
-      <c r="C9" t="s">
-        <v>165</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>247</v>
+      </c>
+      <c r="C11" t="s">
         <v>248</v>
-      </c>
-      <c r="C11" t="s">
-        <v>249</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
@@ -1360,30 +1360,30 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="5"/>
+    <col min="15" max="15" width="12.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -1400,10 +1400,10 @@
         <v>13</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>201</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>202</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>54</v>
@@ -1412,36 +1412,36 @@
         <v>55</v>
       </c>
       <c r="J1" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="Q1" s="8" t="s">
-        <v>211</v>
-      </c>
       <c r="R1" s="8" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>27</v>
@@ -1450,54 +1450,54 @@
         <v>15</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>227</v>
-      </c>
       <c r="F2" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H2" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>218</v>
-      </c>
       <c r="J2" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>239</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>240</v>
       </c>
       <c r="N2" s="5">
         <v>5199779777</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="Q2" s="5">
         <v>512321323</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>27</v>
@@ -1506,31 +1506,31 @@
         <v>15</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>225</v>
-      </c>
       <c r="F3" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>60</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M3" s="5">
         <v>342231</v>
@@ -1539,21 +1539,21 @@
         <v>7205244348</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Q3" s="5">
         <v>6145209478</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>27</v>
@@ -1562,16 +1562,16 @@
         <v>15</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>221</v>
-      </c>
       <c r="G4" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>57</v>
@@ -1580,13 +1580,13 @@
         <v>58</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K4" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="L4" s="5" t="s">
         <v>235</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>236</v>
       </c>
       <c r="M4" s="5">
         <v>208010</v>
@@ -1595,16 +1595,16 @@
         <v>5123213038</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Q4" s="5">
         <v>8794321469</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -1631,29 +1631,29 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -1670,19 +1670,19 @@
         <v>45</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>145</v>
-      </c>
       <c r="I1" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>150</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>151</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>69</v>
@@ -1709,30 +1709,30 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E2" s="5">
         <v>4</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G2" s="6">
         <v>10</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="11"/>
@@ -1758,34 +1758,34 @@
         <v>98091</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G3" t="s">
         <v>148</v>
-      </c>
-      <c r="G3" t="s">
-        <v>149</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3">
         <v>100</v>
       </c>
       <c r="J3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K3" t="s">
         <v>85</v>
@@ -1794,27 +1794,27 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K4" t="s">
         <v>68</v>
@@ -1844,29 +1844,29 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" customWidth="1"/>
-    <col min="10" max="10" width="30.7109375" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" customWidth="1"/>
+    <col min="9" max="9" width="22.44140625" customWidth="1"/>
+    <col min="10" max="10" width="30.6640625" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" customWidth="1"/>
+    <col min="18" max="18" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -1883,16 +1883,16 @@
         <v>45</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>118</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>119</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>16</v>
@@ -1922,36 +1922,36 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E2" s="5">
         <v>2</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="G2" s="11" t="s">
-        <v>126</v>
-      </c>
       <c r="H2" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="I2" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="I2" s="11" t="s">
-        <v>124</v>
-      </c>
       <c r="J2" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>89</v>
@@ -1975,31 +1975,31 @@
         <v>7543</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K3" t="s">
         <v>70</v>
@@ -2008,30 +2008,30 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E4">
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K4" t="s">
         <v>68</v>
@@ -2043,36 +2043,36 @@
         <v>4354312</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G5" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I5" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="J5" t="s">
         <v>136</v>
-      </c>
-      <c r="J5" t="s">
-        <v>137</v>
       </c>
       <c r="K5" t="s">
         <v>89</v>
@@ -2103,29 +2103,29 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -2142,19 +2142,19 @@
         <v>45</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>180</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>181</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>69</v>
@@ -2181,33 +2181,33 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E2" s="5">
         <v>3</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>191</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>192</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>68</v>
@@ -2216,48 +2216,48 @@
         <v>72</v>
       </c>
       <c r="M2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N2" t="s">
         <v>100</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q2">
         <v>567823</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3" t="s">
+        <v>186</v>
+      </c>
+      <c r="G3" t="s">
+        <v>194</v>
+      </c>
+      <c r="H3" t="s">
+        <v>184</v>
+      </c>
+      <c r="J3" t="s">
         <v>187</v>
-      </c>
-      <c r="G3" t="s">
-        <v>195</v>
-      </c>
-      <c r="H3" t="s">
-        <v>185</v>
-      </c>
-      <c r="J3" t="s">
-        <v>188</v>
       </c>
       <c r="K3" t="s">
         <v>96</v>
@@ -2266,33 +2266,33 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E4">
         <v>4</v>
       </c>
       <c r="F4" t="s">
+        <v>192</v>
+      </c>
+      <c r="G4" t="s">
+        <v>183</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="J4" t="s">
         <v>193</v>
-      </c>
-      <c r="G4" t="s">
-        <v>184</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="J4" t="s">
-        <v>194</v>
       </c>
       <c r="K4" t="s">
         <v>70</v>
@@ -2304,36 +2304,36 @@
         <v>6582342</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>85</v>
@@ -2356,28 +2356,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{851E6ACA-76F1-4A5D-873B-D9A5FB72056B}">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -2418,12 +2418,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>67</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>15</v>
@@ -2456,12 +2456,12 @@
         <v>7543</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>87</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>15</v>
@@ -2479,12 +2479,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>15</v>
@@ -2502,12 +2502,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>93</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>15</v>
@@ -2528,12 +2528,12 @@
         <v>4354312</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>95</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>15</v>
@@ -2560,18 +2560,18 @@
         <v>98</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>99</v>
+        <v>252</v>
       </c>
       <c r="L6">
         <v>98091</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>102</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>15</v>
@@ -2598,24 +2598,24 @@
         <v>105</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>106</v>
+        <v>251</v>
       </c>
       <c r="L7">
         <v>7016126</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E8">
         <v>6</v>
@@ -2627,16 +2627,16 @@
         <v>72</v>
       </c>
       <c r="H8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I8" t="s">
         <v>100</v>
       </c>
       <c r="J8" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="K8" s="9" t="s">
         <v>110</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>111</v>
       </c>
       <c r="L8">
         <v>7845255</v>
@@ -2660,24 +2660,24 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="5"/>
-    <col min="6" max="6" width="16.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.85546875" style="6" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="5"/>
-    <col min="11" max="11" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="35.28515625" style="5" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="5"/>
+    <col min="5" max="5" width="9.109375" style="5"/>
+    <col min="6" max="6" width="16.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.88671875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" style="5"/>
+    <col min="11" max="11" width="17.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.33203125" style="5" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>39</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>40</v>
       </c>
@@ -2805,19 +2805,19 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2843,7 +2843,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -2910,17 +2910,17 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2934,7 +2934,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -2942,7 +2942,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -2956,7 +2956,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added option to change the execution sheet at run time
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestData.xlsx
+++ b/src/test/resources/data/TestData.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\java\DataDrivenFramework_v2-sample\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708E64EF-FA5F-436D-8E7A-6463F418AA68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1B48F9-5959-4AEF-95A2-BB171CE320B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
-    <sheet name="AddressesTest" sheetId="11" r:id="rId2"/>
-    <sheet name="JewelryShoesCheckoutTest" sheetId="8" r:id="rId3"/>
-    <sheet name="GiftCardCheckoutTest" sheetId="7" r:id="rId4"/>
-    <sheet name="ComputerCheckoutTest" sheetId="9" r:id="rId5"/>
-    <sheet name="CheckoutProductTest" sheetId="6" r:id="rId6"/>
-    <sheet name="ShoppingCartTest" sheetId="4" r:id="rId7"/>
-    <sheet name="RegisterAccountTest" sheetId="10" r:id="rId8"/>
-    <sheet name="AccountLoginTest" sheetId="3" r:id="rId9"/>
+    <sheet name="Sanity" sheetId="12" r:id="rId1"/>
+    <sheet name="Regression" sheetId="1" r:id="rId2"/>
+    <sheet name="AddressesTest" sheetId="11" r:id="rId3"/>
+    <sheet name="JewelryShoesCheckoutTest" sheetId="8" r:id="rId4"/>
+    <sheet name="GiftCardCheckoutTest" sheetId="7" r:id="rId5"/>
+    <sheet name="ComputerCheckoutTest" sheetId="9" r:id="rId6"/>
+    <sheet name="CheckoutProductTest" sheetId="6" r:id="rId7"/>
+    <sheet name="ShoppingCartTest" sheetId="4" r:id="rId8"/>
+    <sheet name="RegisterAccountTest" sheetId="10" r:id="rId9"/>
+    <sheet name="AccountLoginTest" sheetId="3" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="254">
   <si>
     <t>Description</t>
   </si>
@@ -792,6 +793,9 @@
   </si>
   <si>
     <t>10-2024</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -1168,11 +1172,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0077092-9009-49D9-BD6B-8FE867BDBBFE}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1212,6 +1216,283 @@
         <v>26</v>
       </c>
       <c r="D2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" t="s">
+        <v>253</v>
+      </c>
+      <c r="E6" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D9" t="s">
+        <v>253</v>
+      </c>
+      <c r="E9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>166</v>
+      </c>
+      <c r="C10" t="s">
+        <v>165</v>
+      </c>
+      <c r="D10" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>247</v>
+      </c>
+      <c r="C11" t="s">
+        <v>248</v>
+      </c>
+      <c r="D11" t="s">
+        <v>253</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDAE8DB1-0B2F-47E2-B3A5-A105A60EA0EA}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{448D749D-D972-4CAD-951A-BFDA90EDA3A0}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{883F6DDD-3EE1-4B39-9E02-5A0CEFC957AE}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{026EFFFA-91E6-4EE3-9F4C-011BF1EB8C42}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.44140625" customWidth="1"/>
+    <col min="3" max="3" width="68" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1354,7 +1635,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA62CD38-175E-48A0-A400-D4576F8327A8}">
   <dimension ref="A1:R4"/>
   <sheetViews>
@@ -1623,7 +1904,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD3566D-9000-4AF2-B7E2-9961F511CFC2}">
   <dimension ref="A1:R4"/>
   <sheetViews>
@@ -1836,7 +2117,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{567B4B45-9147-4FB2-ADB3-E350E1D56410}">
   <dimension ref="A1:R5"/>
   <sheetViews>
@@ -2095,7 +2376,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47463942-7A3C-4DBC-89AB-56CFCBFD1840}">
   <dimension ref="A1:R5"/>
   <sheetViews>
@@ -2352,7 +2633,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{851E6ACA-76F1-4A5D-873B-D9A5FB72056B}">
   <dimension ref="A1:M8"/>
   <sheetViews>
@@ -2652,7 +2933,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395827C5-9FCF-499D-AF31-99FCAAB6D481}">
   <dimension ref="A1:L3"/>
   <sheetViews>
@@ -2797,7 +3078,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F4A9D4D-C955-4D50-AFFF-9F62F8F6C2C0}">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -2903,95 +3184,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDAE8DB1-0B2F-47E2-B3A5-A105A60EA0EA}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{448D749D-D972-4CAD-951A-BFDA90EDA3A0}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{883F6DDD-3EE1-4B39-9E02-5A0CEFC957AE}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{026EFFFA-91E6-4EE3-9F4C-011BF1EB8C42}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
-</worksheet>
 </file>
</xml_diff>